<commit_message>
updated study materials y = mem[3];
</commit_message>
<xml_diff>
--- a/Study Materials/UPSParticipantSchedule.xlsx
+++ b/Study Materials/UPSParticipantSchedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="220" windowWidth="21360" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="-280" yWindow="-80" windowWidth="14240" windowHeight="13220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
-  <si>
-    <t>Instructions</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+  <si>
+    <t>Fri. 1:30-2:30</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manya</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>danielcsmyers@gmail.com</t>
@@ -31,79 +35,185 @@
     <t>724-816-7968</t>
   </si>
   <si>
-    <t>12/1/2011 5PM</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>lem81@pitt.edu</t>
+  </si>
+  <si>
+    <t>ams224@gmail.com</t>
+  </si>
+  <si>
+    <t>412-979-1709</t>
+  </si>
+  <si>
+    <t>afinger@andrew.cmu.edu</t>
+  </si>
+  <si>
+    <t>denniso@andrew.cmu.edu</t>
+  </si>
+  <si>
+    <t>917-371-7303</t>
+  </si>
+  <si>
+    <t>yookyung@andrew.cmu.edu</t>
+  </si>
+  <si>
+    <t>rissa543@gmail.com</t>
+  </si>
+  <si>
+    <t>jdotpitts@gmail.com</t>
+  </si>
+  <si>
+    <t>412 304 5680</t>
+  </si>
+  <si>
+    <t>agoginen@andrew.cmu.edu</t>
+  </si>
+  <si>
+    <t>Interview scheduled</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interviewer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note taker</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Email</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phone</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thursday</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thursday</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>apriljianto@gmail.com</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Num</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emailed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Friday</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Friday/Saturday</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Friday/Saturday</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Saturday</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interview</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sat 9-10AM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manya</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jason</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Location</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CIC TBD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sat 1:30-2:30PM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rebecca</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CIC TBD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fri 4:30-5:30</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manya</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Amber</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUPS Lab</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reminder Sent</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Confirmed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send location</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>(408)8320815</t>
-  </si>
-  <si>
-    <t>12/1/2011 5PM</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>lem81@pitt.edu</t>
-  </si>
-  <si>
-    <t>ams224@gmail.com</t>
-  </si>
-  <si>
-    <t>412-979-1709</t>
-  </si>
-  <si>
-    <t>afinger@andrew.cmu.edu</t>
-  </si>
-  <si>
-    <t>denniso@andrew.cmu.edu</t>
-  </si>
-  <si>
-    <t>917-371-7303</t>
-  </si>
-  <si>
-    <t>yookyung@andrew.cmu.edu</t>
-  </si>
-  <si>
-    <t>rissa543@gmail.com</t>
-  </si>
-  <si>
-    <t>jdotpitts@gmail.com</t>
-  </si>
-  <si>
-    <t>412 304 5680</t>
-  </si>
-  <si>
-    <t>agoginen@andrew.cmu.edu</t>
-  </si>
-  <si>
-    <t>Number surveys completed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interview scheduled</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interview location</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interviewer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Note taker</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Email</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Phone</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thurs 6:15-7:15PM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manya</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sauvik</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUPS Lab</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -116,8 +226,13 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -151,9 +266,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,161 +600,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" customWidth="1"/>
+    <col min="9" max="10" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="3">
+        <v>39422</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="2">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
+      <c r="E3" s="3">
+        <v>39422</v>
+      </c>
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>7</v>
       </c>
       <c r="B4">
         <v>6102917695</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3">
+        <v>39422</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>6127019722</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="3">
+        <v>39422</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>7247994355</v>
       </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="C8" s="2">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="3">
+        <v>39422</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>3474948474</v>
       </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="3">
+        <v>39422</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>4088232745</v>
       </c>
-      <c r="C11" t="s">
-        <v>6</v>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="3">
+        <v>39422</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>